<commit_message>
fixed bugs, added an amorization calculator and updated the website.
</commit_message>
<xml_diff>
--- a/reference/Köpa eller hyra_1.xlsx
+++ b/reference/Köpa eller hyra_1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au641277\Documents\GitHub\Verktyg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Verktyg\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD644E4-8227-4857-98DE-FFF33B4985AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25515" windowHeight="14475"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alla år" sheetId="1" r:id="rId1"/>
@@ -43,7 +44,7 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">398339</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +52,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -307,9 +313,6 @@
     <t>Vinster</t>
   </si>
   <si>
-    <t xml:space="preserve">(totalabetalningar*(((1 + r_stocks)^(tid) - 1) / (r_stocks)))-totalabetalningar*tid </t>
-  </si>
-  <si>
     <t>Totala betalningar för att köpa</t>
   </si>
   <si>
@@ -368,12 +371,15 @@
   </si>
   <si>
     <t>rstocks==hyresökning</t>
+  </si>
+  <si>
+    <t>(totalabetalningar*(((1 + r_stocks)^(tid) - 1) / (r_stocks)))-totalabetalningar*tid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="12">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _k_r_-;\-* #,##0.00\ _k_r_-;_-* &quot;-&quot;??\ _k_r_-;_-@_-"/>
@@ -384,9 +390,9 @@
     <numFmt numFmtId="169" formatCode="_-* #,##0.000\ _k_r_-;\-* #,##0.000\ _k_r_-;_-* &quot;-&quot;???\ _k_r_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="_-* #,##0.000000000_-;\-* #,##0.000000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="173" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.0000%"/>
+    <numFmt numFmtId="174" formatCode="0.0000%"/>
+    <numFmt numFmtId="175" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -562,13 +568,12 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -576,35 +581,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -615,11 +615,11 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -629,17 +629,11 @@
     <xf numFmtId="166" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -648,7 +642,8 @@
     </xf>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -667,8 +662,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -984,47 +978,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="102" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="46.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.875" customWidth="1"/>
+    <col min="7" max="7" width="75.8984375" customWidth="1"/>
     <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="12.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="71"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
@@ -1036,7 +1030,7 @@
       <c r="F5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1053,7 +1047,7 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>10000</v>
       </c>
       <c r="H6" t="s">
@@ -1070,7 +1064,7 @@
       <c r="F7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <f>B8*B6</f>
         <v>150000</v>
       </c>
@@ -1093,40 +1087,39 @@
       </c>
       <c r="H8" s="4">
         <f>B71</f>
-        <v>3061.1160154725289</v>
+        <v>4055.8413624190966</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="F9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="49">
+      <c r="G9" s="43">
         <f>SUM(G6:G8)</f>
         <v>160000</v>
       </c>
-      <c r="H9" s="49">
+      <c r="H9" s="43">
         <f>SUM(H6:H8)</f>
-        <v>3061.1160154725289</v>
+        <v>4055.8413624190966</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="80"/>
+      <c r="B10" s="71"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <f>B6*(1-B8)</f>
         <v>850000</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -1136,109 +1129,106 @@
         <f>1-B8</f>
         <v>0.85</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="13">
         <f>SUM(B50:K50)</f>
         <v>162435</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>0.03</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="13">
         <f>SUM(B51:K51)</f>
         <v>100000</v>
       </c>
-      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="13">
         <f>SUM(B52:K52)</f>
         <v>240000</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="5">
         <f>SUM(B69:K69)</f>
-        <v>402220.39764592354</v>
+        <v>532923.97848866601</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>0.3</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="13">
         <f>SUM(B53:K53)</f>
         <v>240000</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <f>SUM(B70:K70)</f>
         <v>120000</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <f>B13*(1-B15)</f>
         <v>2.0999999999999998E-2</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="49">
+      <c r="G16" s="43">
         <f>SUM(G12:G15)</f>
         <v>742435</v>
       </c>
-      <c r="H16" s="65">
+      <c r="H16" s="5">
         <f>SUM(H12:H15)</f>
-        <v>522220.39764592354</v>
+        <v>652923.97848866601</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <v>0.02</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="G18" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="80"/>
+      <c r="B19" s="71"/>
       <c r="F19" s="3" t="s">
         <v>26</v>
       </c>
@@ -1253,9 +1243,9 @@
       <c r="F20" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <f>(B8*B6+G6)*(1+B22)^B25-B8*B6-G6</f>
-        <v>35039.107199161139</v>
+        <v>154744.21716633049</v>
       </c>
       <c r="H20" t="s">
         <v>41</v>
@@ -1265,18 +1255,18 @@
       <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="86">
+      <c r="B21" s="69">
         <v>2.0000001E-2</v>
       </c>
       <c r="C21">
         <v>3048</v>
       </c>
       <c r="F21" t="s">
-        <v>84</v>
-      </c>
-      <c r="G21" s="8">
+        <v>83</v>
+      </c>
+      <c r="G21" s="7">
         <f>B32*(((1+B22)^B25-1)/(B22))-B32*B25</f>
-        <v>71229.074980339035</v>
+        <v>286233.59709596308</v>
       </c>
       <c r="H21" t="s">
         <v>41</v>
@@ -1286,8 +1276,8 @@
       <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="87">
-        <v>0.02</v>
+      <c r="B22" s="70">
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C22">
         <v>3061</v>
@@ -1295,9 +1285,9 @@
       <c r="F22" t="s">
         <v>71</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <f>SUM(B72:K72)+B71*(1+B22)^B25-B71</f>
-        <v>46227.972674024626</v>
+        <v>250234.05988521338</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1310,20 +1300,20 @@
       <c r="F23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="48">
+      <c r="G23" s="42">
         <f>SUM(G20:G22)</f>
-        <v>106268.18217950017</v>
-      </c>
-      <c r="H23" s="49">
+        <v>440977.81426229357</v>
+      </c>
+      <c r="H23" s="43">
         <f>SUM(H22)</f>
-        <v>46227.972674024626</v>
+        <v>250234.05988521338</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="12">
         <v>4.47E-3</v>
       </c>
     </row>
@@ -1342,14 +1332,14 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="80" t="s">
+      <c r="A27" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="80"/>
+      <c r="B27" s="71"/>
       <c r="F27" t="s">
         <v>43</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="5">
         <f>(K48-B6)</f>
         <v>343916.37934412202</v>
       </c>
@@ -1362,12 +1352,12 @@
         <v>9</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="F28" t="s">
-        <v>85</v>
-      </c>
-      <c r="G28" s="6">
+        <v>84</v>
+      </c>
+      <c r="G28" s="5">
         <f>G27-(G27-SUM(B51:K51))*22/30*0.3</f>
         <v>290254.77588841517</v>
       </c>
@@ -1382,10 +1372,10 @@
       <c r="B29" s="1">
         <v>0.01</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G29" s="6"/>
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="5"/>
       <c r="I29" t="s">
         <v>46</v>
       </c>
@@ -1398,9 +1388,9 @@
         <v>24000</v>
       </c>
       <c r="F30" t="s">
-        <v>87</v>
-      </c>
-      <c r="G30" s="6">
+        <v>86</v>
+      </c>
+      <c r="G30" s="5">
         <f>B6*B8</f>
         <v>150000</v>
       </c>
@@ -1415,9 +1405,9 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" s="12">
+        <v>82</v>
+      </c>
+      <c r="B32" s="10">
         <f>B11*B17+B30+B31+B29*B6</f>
         <v>75000</v>
       </c>
@@ -1426,7 +1416,7 @@
       <c r="F33" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G33" s="71">
+      <c r="G33" s="62">
         <f>G28+G29+G30</f>
         <v>440254.77588841517</v>
       </c>
@@ -1436,32 +1426,32 @@
         <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H34" s="66">
+      <c r="H34" s="59">
         <f>K71</f>
-        <v>-3061.1160154725289</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="18">
+        <v>-4055.8413624190966</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="79">
+      <c r="B35" s="4">
         <f>(G37-B106)*(B22-B21)/((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)/12</f>
-        <v>3061.1160154725289</v>
-      </c>
-      <c r="C35" s="69">
+        <v>4055.8413624190966</v>
+      </c>
+      <c r="C35" s="4">
         <f>(G37-B106)*(B22-B21)/((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)/12</f>
-        <v>3061.1160154725289</v>
+        <v>4055.8413624190966</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G35" s="49"/>
+      <c r="G35" s="43"/>
     </row>
     <row r="36" spans="1:12">
       <c r="A36" t="s">
@@ -1482,902 +1472,904 @@
       <c r="F37" t="s">
         <v>50</v>
       </c>
-      <c r="G37" s="72">
+      <c r="G37" s="13">
         <f>G9+G16+G23-G33</f>
-        <v>568448.40629108495</v>
-      </c>
-      <c r="H37" s="72">
+        <v>903158.03837387834</v>
+      </c>
+      <c r="H37" s="13">
         <f>H9+H16+H22+H31+H34</f>
-        <v>568448.37031994818</v>
+        <v>903158.03837387939</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A39" s="85" t="s">
+    <row r="39" spans="1:12" ht="16.2" thickBot="1">
+      <c r="A39" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="85"/>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="85"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="85"/>
-      <c r="H39" s="85"/>
-      <c r="I39" s="85"/>
-      <c r="J39" s="85"/>
-      <c r="K39" s="85"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="76"/>
+      <c r="J39" s="76"/>
+      <c r="K39" s="76"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="43"/>
-      <c r="B40" s="82" t="s">
+      <c r="A40" s="37"/>
+      <c r="B40" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="83"/>
-      <c r="D40" s="83"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="83"/>
-      <c r="H40" s="83"/>
-      <c r="I40" s="83"/>
-      <c r="J40" s="83"/>
-      <c r="K40" s="84"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="74"/>
+      <c r="I40" s="74"/>
+      <c r="J40" s="74"/>
+      <c r="K40" s="75"/>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="51"/>
-      <c r="B41" s="52">
+      <c r="A41" s="45"/>
+      <c r="B41" s="46">
         <v>1</v>
       </c>
-      <c r="C41" s="53">
+      <c r="C41" s="47">
         <v>2</v>
       </c>
-      <c r="D41" s="53">
+      <c r="D41" s="47">
         <v>3</v>
       </c>
-      <c r="E41" s="53">
+      <c r="E41" s="47">
         <v>4</v>
       </c>
-      <c r="F41" s="53">
+      <c r="F41" s="47">
         <v>5</v>
       </c>
-      <c r="G41" s="53">
+      <c r="G41" s="47">
         <v>6</v>
       </c>
-      <c r="H41" s="53">
+      <c r="H41" s="47">
         <v>7</v>
       </c>
-      <c r="I41" s="53">
+      <c r="I41" s="47">
         <v>8</v>
       </c>
-      <c r="J41" s="53">
+      <c r="J41" s="47">
         <v>9</v>
       </c>
-      <c r="K41" s="55">
+      <c r="K41" s="49">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A42" s="51" t="s">
+    <row r="42" spans="1:12" ht="16.2" thickBot="1">
+      <c r="A42" s="45" t="s">
         <v>24</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-      <c r="C42" s="63">
+      <c r="C42" s="57">
         <f>1/(1+$B$23)</f>
         <v>0.98039215686274506</v>
       </c>
-      <c r="D42" s="64">
+      <c r="D42" s="58">
         <f t="shared" ref="D42:K42" si="0">C42/(1+$B$23)</f>
         <v>0.96116878123798533</v>
       </c>
-      <c r="E42" s="64">
+      <c r="E42" s="58">
         <f t="shared" si="0"/>
         <v>0.94232233454704439</v>
       </c>
-      <c r="F42" s="64">
+      <c r="F42" s="58">
         <f t="shared" si="0"/>
         <v>0.92384542602651409</v>
       </c>
-      <c r="G42" s="64">
+      <c r="G42" s="58">
         <f t="shared" si="0"/>
         <v>0.90573080982991572</v>
       </c>
-      <c r="H42" s="64">
+      <c r="H42" s="58">
         <f t="shared" si="0"/>
         <v>0.88797138218619187</v>
       </c>
-      <c r="I42" s="64">
+      <c r="I42" s="58">
         <f t="shared" si="0"/>
         <v>0.87056017861391355</v>
       </c>
-      <c r="J42" s="64">
+      <c r="J42" s="58">
         <f t="shared" si="0"/>
         <v>0.85349037119011129</v>
       </c>
-      <c r="K42" s="64">
+      <c r="K42" s="58">
         <f t="shared" si="0"/>
         <v>0.83675526587265814</v>
       </c>
-      <c r="L42" s="64"/>
-    </row>
-    <row r="43" spans="1:12" s="11" customFormat="1">
-      <c r="A43" s="32" t="s">
+      <c r="L42" s="58"/>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="34"/>
-    </row>
-    <row r="44" spans="1:12" s="11" customFormat="1">
-      <c r="A44" s="35" t="s">
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="28"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="36">
+      <c r="B44" s="30">
         <f t="shared" ref="B44:K44" si="1">$B$17*$B$11</f>
         <v>17000</v>
       </c>
-      <c r="C44" s="36">
+      <c r="C44" s="30">
         <f t="shared" si="1"/>
         <v>17000</v>
       </c>
-      <c r="D44" s="36">
+      <c r="D44" s="30">
         <f t="shared" si="1"/>
         <v>17000</v>
       </c>
-      <c r="E44" s="36">
+      <c r="E44" s="30">
         <f t="shared" si="1"/>
         <v>17000</v>
       </c>
-      <c r="F44" s="36">
+      <c r="F44" s="30">
         <f t="shared" si="1"/>
         <v>17000</v>
       </c>
-      <c r="G44" s="36">
+      <c r="G44" s="30">
         <f t="shared" si="1"/>
         <v>17000</v>
       </c>
-      <c r="H44" s="36">
+      <c r="H44" s="30">
         <f t="shared" si="1"/>
         <v>17000</v>
       </c>
-      <c r="I44" s="36">
+      <c r="I44" s="30">
         <f t="shared" si="1"/>
         <v>17000</v>
       </c>
-      <c r="J44" s="36">
+      <c r="J44" s="30">
         <f t="shared" si="1"/>
         <v>17000</v>
       </c>
-      <c r="K44" s="37">
+      <c r="K44" s="31">
         <f t="shared" si="1"/>
         <v>17000</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="11" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A45" s="35" t="s">
+    <row r="45" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A45" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="38">
+      <c r="B45" s="32">
         <f>B11</f>
         <v>850000</v>
       </c>
-      <c r="C45" s="39">
+      <c r="C45" s="33">
         <f t="shared" ref="C45:K45" si="2">B45-B44</f>
         <v>833000</v>
       </c>
-      <c r="D45" s="39">
+      <c r="D45" s="33">
         <f t="shared" si="2"/>
         <v>816000</v>
       </c>
-      <c r="E45" s="39">
+      <c r="E45" s="33">
         <f t="shared" si="2"/>
         <v>799000</v>
       </c>
-      <c r="F45" s="39">
+      <c r="F45" s="33">
         <f t="shared" si="2"/>
         <v>782000</v>
       </c>
-      <c r="G45" s="39">
+      <c r="G45" s="33">
         <f t="shared" si="2"/>
         <v>765000</v>
       </c>
-      <c r="H45" s="39">
+      <c r="H45" s="33">
         <f t="shared" si="2"/>
         <v>748000</v>
       </c>
-      <c r="I45" s="39">
+      <c r="I45" s="33">
         <f t="shared" si="2"/>
         <v>731000</v>
       </c>
-      <c r="J45" s="39">
+      <c r="J45" s="33">
         <f t="shared" si="2"/>
         <v>714000</v>
       </c>
-      <c r="K45" s="40">
+      <c r="K45" s="34">
         <f t="shared" si="2"/>
         <v>697000</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="11" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A46" s="35"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="40"/>
-    </row>
-    <row r="47" spans="1:12" s="11" customFormat="1">
-      <c r="A47" s="35" t="s">
+    <row r="46" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A46" s="29"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="34"/>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B47" s="41">
+      <c r="B47" s="35">
         <f t="shared" ref="B47:K47" si="3">B45/$B$6</f>
         <v>0.85</v>
       </c>
-      <c r="C47" s="41">
+      <c r="C47" s="35">
         <f t="shared" si="3"/>
         <v>0.83299999999999996</v>
       </c>
-      <c r="D47" s="41">
+      <c r="D47" s="35">
         <f t="shared" si="3"/>
         <v>0.81599999999999995</v>
       </c>
-      <c r="E47" s="41">
+      <c r="E47" s="35">
         <f t="shared" si="3"/>
         <v>0.79900000000000004</v>
       </c>
-      <c r="F47" s="41">
+      <c r="F47" s="35">
         <f t="shared" si="3"/>
         <v>0.78200000000000003</v>
       </c>
-      <c r="G47" s="41">
+      <c r="G47" s="35">
         <f t="shared" si="3"/>
         <v>0.76500000000000001</v>
       </c>
-      <c r="H47" s="41">
+      <c r="H47" s="35">
         <f t="shared" si="3"/>
         <v>0.748</v>
       </c>
-      <c r="I47" s="41">
+      <c r="I47" s="35">
         <f t="shared" si="3"/>
         <v>0.73099999999999998</v>
       </c>
-      <c r="J47" s="41">
+      <c r="J47" s="35">
         <f t="shared" si="3"/>
         <v>0.71399999999999997</v>
       </c>
-      <c r="K47" s="42">
+      <c r="K47" s="36">
         <f t="shared" si="3"/>
         <v>0.69699999999999995</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="11" customFormat="1">
-      <c r="A48" s="35" t="s">
+    <row r="48" spans="1:12">
+      <c r="A48" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B48" s="38">
+      <c r="B48" s="32">
         <f>B6*(1+B20)</f>
         <v>1030000</v>
       </c>
-      <c r="C48" s="38">
+      <c r="C48" s="32">
         <f t="shared" ref="C48:K48" si="4">B48*(1+$B$20)</f>
         <v>1060900</v>
       </c>
-      <c r="D48" s="38">
+      <c r="D48" s="32">
         <f t="shared" si="4"/>
         <v>1092727</v>
       </c>
-      <c r="E48" s="38">
+      <c r="E48" s="32">
         <f t="shared" si="4"/>
         <v>1125508.81</v>
       </c>
-      <c r="F48" s="38">
+      <c r="F48" s="32">
         <f t="shared" si="4"/>
         <v>1159274.0743</v>
       </c>
-      <c r="G48" s="38">
+      <c r="G48" s="32">
         <f t="shared" si="4"/>
         <v>1194052.2965289999</v>
       </c>
-      <c r="H48" s="38">
+      <c r="H48" s="32">
         <f t="shared" si="4"/>
         <v>1229873.86542487</v>
       </c>
-      <c r="I48" s="38">
+      <c r="I48" s="32">
         <f t="shared" si="4"/>
         <v>1266770.0813876162</v>
       </c>
-      <c r="J48" s="38">
+      <c r="J48" s="32">
         <f t="shared" si="4"/>
         <v>1304773.1838292447</v>
       </c>
-      <c r="K48" s="56">
+      <c r="K48" s="50">
         <f t="shared" si="4"/>
         <v>1343916.379344122</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="11" customFormat="1">
-      <c r="A49" s="57" t="s">
+    <row r="49" spans="1:12">
+      <c r="A49" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
-      <c r="J49" s="19"/>
-      <c r="K49" s="24"/>
-    </row>
-    <row r="50" spans="1:12" s="11" customFormat="1">
-      <c r="A50" s="21" t="s">
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="18"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B50" s="20">
+      <c r="B50" s="15">
         <f>B45*$B$16</f>
         <v>17849.999999999996</v>
       </c>
-      <c r="C50" s="20">
+      <c r="C50" s="15">
         <f t="shared" ref="C50:K50" si="5">C45*$B$16</f>
         <v>17493</v>
       </c>
-      <c r="D50" s="20">
+      <c r="D50" s="15">
         <f t="shared" si="5"/>
         <v>17136</v>
       </c>
-      <c r="E50" s="20">
+      <c r="E50" s="15">
         <f t="shared" si="5"/>
         <v>16779</v>
       </c>
-      <c r="F50" s="20">
+      <c r="F50" s="15">
         <f t="shared" si="5"/>
         <v>16422</v>
       </c>
-      <c r="G50" s="20">
+      <c r="G50" s="15">
         <f t="shared" si="5"/>
         <v>16064.999999999998</v>
       </c>
-      <c r="H50" s="20">
+      <c r="H50" s="15">
         <f t="shared" si="5"/>
         <v>15707.999999999998</v>
       </c>
-      <c r="I50" s="20">
+      <c r="I50" s="15">
         <f t="shared" si="5"/>
         <v>15350.999999999998</v>
       </c>
-      <c r="J50" s="20">
+      <c r="J50" s="15">
         <f t="shared" si="5"/>
         <v>14993.999999999998</v>
       </c>
-      <c r="K50" s="22">
+      <c r="K50" s="17">
         <f t="shared" si="5"/>
         <v>14636.999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="11" customFormat="1">
-      <c r="A51" s="23" t="s">
+    <row r="51" spans="1:12">
+      <c r="A51" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="19">
+      <c r="B51" s="14">
         <f>$B$6*$B$29</f>
         <v>10000</v>
       </c>
-      <c r="C51" s="19">
+      <c r="C51" s="14">
         <f t="shared" ref="C51:K51" si="6">$B$6*$B$29</f>
         <v>10000</v>
       </c>
-      <c r="D51" s="19">
+      <c r="D51" s="14">
         <f t="shared" si="6"/>
         <v>10000</v>
       </c>
-      <c r="E51" s="19">
+      <c r="E51" s="14">
         <f t="shared" si="6"/>
         <v>10000</v>
       </c>
-      <c r="F51" s="19">
+      <c r="F51" s="14">
         <f t="shared" si="6"/>
         <v>10000</v>
       </c>
-      <c r="G51" s="19">
+      <c r="G51" s="14">
         <f t="shared" si="6"/>
         <v>10000</v>
       </c>
-      <c r="H51" s="19">
+      <c r="H51" s="14">
         <f t="shared" si="6"/>
         <v>10000</v>
       </c>
-      <c r="I51" s="19">
+      <c r="I51" s="14">
         <f t="shared" si="6"/>
         <v>10000</v>
       </c>
-      <c r="J51" s="19">
+      <c r="J51" s="14">
         <f t="shared" si="6"/>
         <v>10000</v>
       </c>
-      <c r="K51" s="19">
+      <c r="K51" s="14">
         <f t="shared" si="6"/>
         <v>10000</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="11" customFormat="1">
-      <c r="A52" s="23" t="s">
+    <row r="52" spans="1:12">
+      <c r="A52" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B52" s="19">
+      <c r="B52" s="14">
         <f>$B$30</f>
         <v>24000</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="14">
         <f t="shared" ref="C52:K52" si="7">$B$30</f>
         <v>24000</v>
       </c>
-      <c r="D52" s="19">
+      <c r="D52" s="14">
         <f t="shared" si="7"/>
         <v>24000</v>
       </c>
-      <c r="E52" s="19">
+      <c r="E52" s="14">
         <f t="shared" si="7"/>
         <v>24000</v>
       </c>
-      <c r="F52" s="19">
+      <c r="F52" s="14">
         <f t="shared" si="7"/>
         <v>24000</v>
       </c>
-      <c r="G52" s="19">
+      <c r="G52" s="14">
         <f t="shared" si="7"/>
         <v>24000</v>
       </c>
-      <c r="H52" s="19">
+      <c r="H52" s="14">
         <f t="shared" si="7"/>
         <v>24000</v>
       </c>
-      <c r="I52" s="19">
+      <c r="I52" s="14">
         <f t="shared" si="7"/>
         <v>24000</v>
       </c>
-      <c r="J52" s="19">
+      <c r="J52" s="14">
         <f t="shared" si="7"/>
         <v>24000</v>
       </c>
-      <c r="K52" s="24">
+      <c r="K52" s="18">
         <f t="shared" si="7"/>
         <v>24000</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="11" customFormat="1">
-      <c r="A53" s="23" t="s">
+    <row r="53" spans="1:12">
+      <c r="A53" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B53" s="19">
+      <c r="B53" s="14">
         <f>$B$31</f>
         <v>24000</v>
       </c>
-      <c r="C53" s="19">
+      <c r="C53" s="14">
         <f t="shared" ref="C53:K53" si="8">$B$31</f>
         <v>24000</v>
       </c>
-      <c r="D53" s="19">
+      <c r="D53" s="14">
         <f t="shared" si="8"/>
         <v>24000</v>
       </c>
-      <c r="E53" s="19">
+      <c r="E53" s="14">
         <f t="shared" si="8"/>
         <v>24000</v>
       </c>
-      <c r="F53" s="19">
+      <c r="F53" s="14">
         <f t="shared" si="8"/>
         <v>24000</v>
       </c>
-      <c r="G53" s="19">
+      <c r="G53" s="14">
         <f t="shared" si="8"/>
         <v>24000</v>
       </c>
-      <c r="H53" s="19">
+      <c r="H53" s="14">
         <f t="shared" si="8"/>
         <v>24000</v>
       </c>
-      <c r="I53" s="19">
+      <c r="I53" s="14">
         <f t="shared" si="8"/>
         <v>24000</v>
       </c>
-      <c r="J53" s="19">
+      <c r="J53" s="14">
         <f t="shared" si="8"/>
         <v>24000</v>
       </c>
-      <c r="K53" s="19">
+      <c r="K53" s="14">
         <f t="shared" si="8"/>
         <v>24000</v>
       </c>
     </row>
-    <row r="54" spans="1:12" s="11" customFormat="1">
-      <c r="A54" s="23"/>
-      <c r="B54" s="19">
+    <row r="54" spans="1:12">
+      <c r="A54" s="16"/>
+      <c r="B54" s="14">
         <f>SUM(B50:B53)</f>
         <v>75850</v>
       </c>
-      <c r="C54" s="19">
+      <c r="C54" s="14">
         <f t="shared" ref="C54:K54" si="9">SUM(C50:C53)</f>
         <v>75493</v>
       </c>
-      <c r="D54" s="19">
+      <c r="D54" s="14">
         <f t="shared" si="9"/>
         <v>75136</v>
       </c>
-      <c r="E54" s="19">
+      <c r="E54" s="14">
         <f t="shared" si="9"/>
         <v>74779</v>
       </c>
-      <c r="F54" s="19">
+      <c r="F54" s="14">
         <f t="shared" si="9"/>
         <v>74422</v>
       </c>
-      <c r="G54" s="19">
+      <c r="G54" s="14">
         <f t="shared" si="9"/>
         <v>74065</v>
       </c>
-      <c r="H54" s="19">
+      <c r="H54" s="14">
         <f t="shared" si="9"/>
         <v>73708</v>
       </c>
-      <c r="I54" s="19">
+      <c r="I54" s="14">
         <f t="shared" si="9"/>
         <v>73351</v>
       </c>
-      <c r="J54" s="19">
+      <c r="J54" s="14">
         <f t="shared" si="9"/>
         <v>72994</v>
       </c>
-      <c r="K54" s="19">
+      <c r="K54" s="14">
         <f t="shared" si="9"/>
         <v>72637</v>
       </c>
     </row>
-    <row r="55" spans="1:12" s="11" customFormat="1">
-      <c r="A55" s="58" t="s">
+    <row r="55" spans="1:12">
+      <c r="A55" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="59"/>
-    </row>
-    <row r="56" spans="1:12" s="11" customFormat="1">
-      <c r="A56" s="60" t="s">
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="53"/>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="B56" s="50">
+      <c r="B56" s="44">
         <f>B6*B28</f>
+        <v>10000</v>
+      </c>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="55">
+        <f>K48*B28</f>
+        <v>13439.163793441221</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="44">
+        <v>150000</v>
+      </c>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="55">
+        <v>-150000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="21"/>
+      <c r="C58" s="48"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="48"/>
+      <c r="F58" s="48"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="48"/>
+      <c r="I58" s="48"/>
+      <c r="J58" s="48"/>
+      <c r="K58" s="22"/>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" s="21">
+        <f>($B$6*$B$8+$B$56)*(1+$B$22)</f>
+        <v>171200</v>
+      </c>
+      <c r="C59" s="21">
+        <f t="shared" ref="C59:K59" si="10">(B59-B62)*(1+$B$22)</f>
+        <v>183184</v>
+      </c>
+      <c r="D59" s="21">
+        <f t="shared" si="10"/>
+        <v>196006.88</v>
+      </c>
+      <c r="E59" s="21">
+        <f t="shared" si="10"/>
+        <v>209727.3616</v>
+      </c>
+      <c r="F59" s="21">
+        <f t="shared" si="10"/>
+        <v>224408.27691200003</v>
+      </c>
+      <c r="G59" s="21">
+        <f t="shared" si="10"/>
+        <v>240116.85629584006</v>
+      </c>
+      <c r="H59" s="21">
+        <f t="shared" si="10"/>
+        <v>256925.03623654888</v>
+      </c>
+      <c r="I59" s="21">
+        <f t="shared" si="10"/>
+        <v>274909.78877310734</v>
+      </c>
+      <c r="J59" s="21">
+        <f t="shared" si="10"/>
+        <v>294153.47398722486</v>
+      </c>
+      <c r="K59" s="21">
+        <f t="shared" si="10"/>
+        <v>314744.21716633061</v>
+      </c>
+      <c r="L59" s="5">
+        <f>K59-160000</f>
+        <v>154744.21716633061</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="21"/>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="22"/>
+    </row>
+    <row r="62" spans="1:12" ht="16.2" thickBot="1">
+      <c r="A62" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="24"/>
+      <c r="H62" s="24"/>
+      <c r="I62" s="24"/>
+      <c r="J62" s="24"/>
+      <c r="K62" s="25"/>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="B63" s="60"/>
+      <c r="C63" s="61"/>
+    </row>
+    <row r="65" spans="1:11" ht="16.2" thickBot="1">
+      <c r="A65" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="72"/>
+      <c r="C65" s="72"/>
+      <c r="D65" s="72"/>
+      <c r="E65" s="72"/>
+      <c r="F65" s="72"/>
+      <c r="G65" s="72"/>
+      <c r="H65" s="72"/>
+      <c r="I65" s="72"/>
+      <c r="J65" s="72"/>
+      <c r="K65" s="72"/>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="37"/>
+      <c r="B66" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="25"/>
-      <c r="I56" s="25"/>
-      <c r="J56" s="25"/>
-      <c r="K56" s="61">
-        <f>K48*B28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" s="11" customFormat="1">
-      <c r="A57" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57" s="50">
-        <v>150000</v>
-      </c>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
-      <c r="I57" s="25"/>
-      <c r="J57" s="25"/>
-      <c r="K57" s="61">
-        <v>-150000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" s="11" customFormat="1">
-      <c r="A58" s="62" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="27"/>
-      <c r="C58" s="54"/>
-      <c r="D58" s="54"/>
-      <c r="E58" s="54"/>
-      <c r="F58" s="54"/>
-      <c r="G58" s="54"/>
-      <c r="H58" s="54"/>
-      <c r="I58" s="54"/>
-      <c r="J58" s="54"/>
-      <c r="K58" s="28"/>
-    </row>
-    <row r="59" spans="1:12" s="11" customFormat="1">
-      <c r="A59" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B59" s="27">
-        <f>($B$6*$B$8+$B$56)*(1+$B$22)</f>
-        <v>153000</v>
-      </c>
-      <c r="C59" s="27">
-        <f t="shared" ref="C59:K59" si="10">(B59-B62)*(1+$B$22)</f>
-        <v>156060</v>
-      </c>
-      <c r="D59" s="27">
-        <f t="shared" si="10"/>
-        <v>159181.20000000001</v>
-      </c>
-      <c r="E59" s="27">
-        <f t="shared" si="10"/>
-        <v>162364.82400000002</v>
-      </c>
-      <c r="F59" s="27">
-        <f t="shared" si="10"/>
-        <v>165612.12048000001</v>
-      </c>
-      <c r="G59" s="27">
-        <f t="shared" si="10"/>
-        <v>168924.36288960002</v>
-      </c>
-      <c r="H59" s="27">
-        <f t="shared" si="10"/>
-        <v>172302.85014739202</v>
-      </c>
-      <c r="I59" s="27">
-        <f t="shared" si="10"/>
-        <v>175748.90715033986</v>
-      </c>
-      <c r="J59" s="27">
-        <f t="shared" si="10"/>
-        <v>179263.88529334666</v>
-      </c>
-      <c r="K59" s="27">
-        <f t="shared" si="10"/>
-        <v>182849.16299921359</v>
-      </c>
-      <c r="L59" s="16"/>
-    </row>
-    <row r="60" spans="1:12" s="11" customFormat="1">
-      <c r="A60" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B60" s="27"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
-      <c r="G60" s="27"/>
-      <c r="H60" s="27"/>
-      <c r="I60" s="27"/>
-      <c r="J60" s="27"/>
-      <c r="K60" s="27"/>
-    </row>
-    <row r="61" spans="1:12" s="11" customFormat="1">
-      <c r="A61" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
-      <c r="I61" s="27"/>
-      <c r="J61" s="27"/>
-      <c r="K61" s="28"/>
-    </row>
-    <row r="62" spans="1:12" s="11" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A62" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B62" s="30"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="30"/>
-      <c r="J62" s="30"/>
-      <c r="K62" s="31"/>
-    </row>
-    <row r="63" spans="1:12" s="11" customFormat="1">
-      <c r="B63" s="67"/>
-      <c r="C63" s="68"/>
-    </row>
-    <row r="64" spans="1:12" s="11" customFormat="1"/>
-    <row r="65" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A65" s="81" t="s">
-        <v>59</v>
-      </c>
-      <c r="B65" s="81"/>
-      <c r="C65" s="81"/>
-      <c r="D65" s="81"/>
-      <c r="E65" s="81"/>
-      <c r="F65" s="81"/>
-      <c r="G65" s="81"/>
-      <c r="H65" s="81"/>
-      <c r="I65" s="81"/>
-      <c r="J65" s="81"/>
-      <c r="K65" s="81"/>
-    </row>
-    <row r="66" spans="1:11">
-      <c r="A66" s="43"/>
-      <c r="B66" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="C66" s="83"/>
-      <c r="D66" s="83"/>
-      <c r="E66" s="83"/>
-      <c r="F66" s="83"/>
-      <c r="G66" s="83"/>
-      <c r="H66" s="83"/>
-      <c r="I66" s="83"/>
-      <c r="J66" s="83"/>
-      <c r="K66" s="84"/>
-    </row>
-    <row r="67" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A67" s="44"/>
-      <c r="B67" s="47">
+      <c r="C66" s="74"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
+      <c r="F66" s="74"/>
+      <c r="G66" s="74"/>
+      <c r="H66" s="74"/>
+      <c r="I66" s="74"/>
+      <c r="J66" s="74"/>
+      <c r="K66" s="75"/>
+    </row>
+    <row r="67" spans="1:11" ht="16.2" thickBot="1">
+      <c r="A67" s="38"/>
+      <c r="B67" s="41">
         <v>1</v>
       </c>
-      <c r="C67" s="45">
+      <c r="C67" s="39">
         <v>2</v>
       </c>
-      <c r="D67" s="45">
+      <c r="D67" s="39">
         <v>3</v>
       </c>
-      <c r="E67" s="45">
+      <c r="E67" s="39">
         <v>4</v>
       </c>
-      <c r="F67" s="45">
+      <c r="F67" s="39">
         <v>5</v>
       </c>
-      <c r="G67" s="45">
+      <c r="G67" s="39">
         <v>6</v>
       </c>
-      <c r="H67" s="45">
+      <c r="H67" s="39">
         <v>7</v>
       </c>
-      <c r="I67" s="45">
+      <c r="I67" s="39">
         <v>8</v>
       </c>
-      <c r="J67" s="45">
+      <c r="J67" s="39">
         <v>9</v>
       </c>
-      <c r="K67" s="46">
+      <c r="K67" s="40">
         <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="57" t="s">
+      <c r="A68" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="B68" s="53"/>
-      <c r="C68" s="53"/>
-      <c r="D68" s="53"/>
-      <c r="E68" s="53"/>
-      <c r="F68" s="53"/>
-      <c r="G68" s="53"/>
-      <c r="H68" s="53"/>
-      <c r="I68" s="53"/>
-      <c r="J68" s="53"/>
-      <c r="K68" s="53"/>
+      <c r="B68" s="47"/>
+      <c r="C68" s="47"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="47"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="47"/>
+      <c r="I68" s="47"/>
+      <c r="J68" s="47"/>
+      <c r="K68" s="47"/>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>55</v>
       </c>
-      <c r="B69" s="6">
+      <c r="B69" s="5">
         <f>B35*12</f>
-        <v>36733.392185670345</v>
-      </c>
-      <c r="C69" s="6">
+        <v>48670.096349029162</v>
+      </c>
+      <c r="C69" s="5">
         <f>B69*(1+$B$21)</f>
-        <v>37468.060066117148</v>
-      </c>
-      <c r="D69" s="6">
+        <v>49643.498324679844</v>
+      </c>
+      <c r="D69" s="5">
         <f t="shared" ref="D69:K69" si="11">C69*(1+$B$21)</f>
-        <v>38217.421304907555</v>
-      </c>
-      <c r="E69" s="6">
+        <v>50636.368340816945</v>
+      </c>
+      <c r="E69" s="5">
         <f t="shared" si="11"/>
-        <v>38981.76976922313</v>
-      </c>
-      <c r="F69" s="6">
+        <v>51649.095758269657</v>
+      </c>
+      <c r="F69" s="5">
         <f t="shared" si="11"/>
-        <v>39761.405203589369</v>
-      </c>
-      <c r="G69" s="6">
+        <v>52682.077725084149</v>
+      </c>
+      <c r="G69" s="5">
         <f t="shared" si="11"/>
-        <v>40556.633347422568</v>
-      </c>
-      <c r="H69" s="6">
+        <v>53735.719332267916</v>
+      </c>
+      <c r="H69" s="5">
         <f t="shared" si="11"/>
-        <v>41367.766054927655</v>
-      </c>
-      <c r="I69" s="6">
+        <v>54810.433772648998</v>
+      </c>
+      <c r="I69" s="5">
         <f t="shared" si="11"/>
-        <v>42195.121417393981</v>
-      </c>
-      <c r="J69" s="6">
+        <v>55906.642502912415</v>
+      </c>
+      <c r="J69" s="5">
         <f t="shared" si="11"/>
-        <v>43039.023887936986</v>
-      </c>
-      <c r="K69" s="6">
+        <v>57024.775408877314</v>
+      </c>
+      <c r="K69" s="5">
         <f t="shared" si="11"/>
-        <v>43899.804408734752</v>
+        <v>58165.270974079642</v>
       </c>
     </row>
     <row r="70" spans="1:11">
       <c r="A70" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="6">
+      <c r="B70" s="5">
         <f>B37</f>
         <v>12000</v>
       </c>
-      <c r="C70" s="6">
+      <c r="C70" s="5">
         <f>B70</f>
         <v>12000</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D70" s="5">
         <f t="shared" ref="D70:K70" si="12">C70</f>
         <v>12000</v>
       </c>
-      <c r="E70" s="6">
+      <c r="E70" s="5">
         <f t="shared" si="12"/>
         <v>12000</v>
       </c>
-      <c r="F70" s="6">
+      <c r="F70" s="5">
         <f t="shared" si="12"/>
         <v>12000</v>
       </c>
-      <c r="G70" s="6">
+      <c r="G70" s="5">
         <f t="shared" si="12"/>
         <v>12000</v>
       </c>
-      <c r="H70" s="6">
+      <c r="H70" s="5">
         <f t="shared" si="12"/>
         <v>12000</v>
       </c>
-      <c r="I70" s="6">
+      <c r="I70" s="5">
         <f t="shared" si="12"/>
         <v>12000</v>
       </c>
-      <c r="J70" s="6">
+      <c r="J70" s="5">
         <f t="shared" si="12"/>
         <v>12000</v>
       </c>
-      <c r="K70" s="6">
+      <c r="K70" s="5">
         <f t="shared" si="12"/>
         <v>12000</v>
       </c>
@@ -2388,56 +2380,56 @@
       </c>
       <c r="B71" s="4">
         <f>B36*B35</f>
-        <v>3061.1160154725289</v>
+        <v>4055.8413624190966</v>
       </c>
       <c r="K71">
         <f>-B71</f>
-        <v>-3061.1160154725289</v>
+        <v>-4055.8413624190966</v>
       </c>
     </row>
     <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>70</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="5">
         <f>(B69)*(1+$B$22)^($B$25-B67+1)-(B69)</f>
-        <v>8044.4079161408226</v>
-      </c>
-      <c r="C72" s="6">
+        <v>47071.34974337749</v>
+      </c>
+      <c r="C72" s="5">
         <f t="shared" ref="C72:K72" si="13">(C69)*(1+$B$22)^($B$25-C67+1)-(C69)</f>
-        <v>7309.7400795938229</v>
-      </c>
-      <c r="D72" s="6">
+        <v>41624.048507092339</v>
+      </c>
+      <c r="D72" s="5">
         <f t="shared" si="13"/>
-        <v>6560.3788847032265</v>
-      </c>
-      <c r="E72" s="6">
+        <v>36366.339939253317</v>
+      </c>
+      <c r="E72" s="5">
         <f t="shared" si="13"/>
-        <v>5796.0304642874544</v>
-      </c>
-      <c r="F72" s="6">
+        <v>31288.065487220418</v>
+      </c>
+      <c r="F72" s="5">
         <f t="shared" si="13"/>
-        <v>5016.3950738210333</v>
-      </c>
-      <c r="G72" s="6">
+        <v>26379.515315417753</v>
+      </c>
+      <c r="G72" s="5">
         <f t="shared" si="13"/>
-        <v>4221.1669738876444</v>
-      </c>
-      <c r="H72" s="6">
+        <v>21631.406817613904</v>
+      </c>
+      <c r="H72" s="5">
         <f t="shared" si="13"/>
-        <v>3410.0343102823608</v>
-      </c>
-      <c r="I72" s="6">
+        <v>17034.864122908555</v>
+      </c>
+      <c r="I72" s="5">
         <f t="shared" si="13"/>
-        <v>2582.6789917158458</v>
-      </c>
-      <c r="J72" s="6">
+        <v>12581.398548782927</v>
+      </c>
+      <c r="J72" s="5">
         <f t="shared" si="13"/>
-        <v>1738.7765650726506</v>
-      </c>
-      <c r="K72" s="6">
+        <v>8262.8899567463232</v>
+      </c>
+      <c r="K72" s="5">
         <f t="shared" si="13"/>
-        <v>877.99608817469561</v>
+        <v>4071.5689681855802</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -2455,47 +2447,47 @@
       <c r="A75" t="s">
         <v>26</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="5">
         <f>B69*((1+B22)*(-1+(1+B22))*((1+B22)^B25-(1+B21)^B25))/(B22*(-1+(1+B22)-B21))</f>
-        <v>447778.04673245124</v>
-      </c>
-      <c r="C75" s="6">
+        <v>779235.42589526344</v>
+      </c>
+      <c r="C75" s="5">
         <f>B71*(1+B22)^B25-B71</f>
-        <v>670.36732634506825</v>
-      </c>
-      <c r="D75" s="6">
+        <v>3922.6124786147898</v>
+      </c>
+      <c r="D75" s="5">
         <f>C75+B75</f>
-        <v>448448.4140587963</v>
+        <v>783158.03837387823</v>
       </c>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" t="s">
         <v>72</v>
       </c>
-      <c r="B76" s="76">
+      <c r="B76" s="66">
         <f>B69*(1-(1+B21)^10)/(1-(1+B21))</f>
-        <v>402220.39764592296</v>
-      </c>
-      <c r="D76" s="6"/>
+        <v>532923.97848866542</v>
+      </c>
+      <c r="D76" s="5"/>
     </row>
     <row r="77" spans="1:11">
-      <c r="B77" s="6">
+      <c r="B77" s="5">
         <f>B75-B76</f>
-        <v>45557.649086528283</v>
-      </c>
-      <c r="C77" s="6"/>
+        <v>246311.44740659802</v>
+      </c>
+      <c r="C77" s="5"/>
     </row>
     <row r="79" spans="1:11">
       <c r="A79" t="s">
         <v>73</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="5">
         <f>B75+C75-B76</f>
-        <v>46228.016412873345</v>
+        <v>250234.0598852128</v>
       </c>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="6"/>
+      <c r="A80" s="5"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="3" t="s">
@@ -2514,11 +2506,11 @@
       </c>
       <c r="B82" s="4">
         <f>B69*(1+B22)*((1+B22)^B25-(1+B21)^B25)/(B22-B21)</f>
-        <v>447778.03896473994</v>
+        <v>779235.42589526367</v>
       </c>
       <c r="C82" s="4">
         <f>B71*(1+B22)^B25</f>
-        <v>3731.4833418175972</v>
+        <v>7978.4538410338864</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2527,33 +2519,33 @@
       </c>
       <c r="B83" s="4">
         <f>B69*((1-(1+B21)^B25))/(1-(1+B21))</f>
-        <v>402220.39764592296</v>
-      </c>
-      <c r="C83" s="6">
+        <v>532923.97848866542</v>
+      </c>
+      <c r="C83" s="5">
         <f>B71</f>
-        <v>3061.1160154725289</v>
+        <v>4055.8413624190966</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>78</v>
       </c>
-      <c r="B84" s="77">
+      <c r="B84" s="67">
         <f>B82-B83</f>
-        <v>45557.641318816983</v>
-      </c>
-      <c r="C84" s="6">
+        <v>246311.44740659825</v>
+      </c>
+      <c r="C84" s="5">
         <f>C82-C83</f>
-        <v>670.36732634506825</v>
+        <v>3922.6124786147898</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>77</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="5">
         <f>B84+C84</f>
-        <v>46228.008645162052</v>
+        <v>250234.05988521304</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2568,34 +2560,34 @@
       <c r="A89" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B89" s="48"/>
+      <c r="B89" s="42"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B90" s="12"/>
+      <c r="B90" s="10"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>88</v>
-      </c>
-      <c r="B91" s="12">
+        <v>87</v>
+      </c>
+      <c r="B91" s="10">
         <f>B37*B25</f>
         <v>120000</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>89</v>
-      </c>
-      <c r="B92" s="6"/>
+        <v>88</v>
+      </c>
+      <c r="B92" s="5"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>93</v>
-      </c>
-      <c r="B93" s="6">
+        <v>92</v>
+      </c>
+      <c r="B93" s="5">
         <f>B91+B92</f>
         <v>120000</v>
       </c>
@@ -2607,75 +2599,75 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>90</v>
-      </c>
-      <c r="B95" s="6">
+        <v>89</v>
+      </c>
+      <c r="B95" s="5">
         <f>B69*(1+B22)*((1+B22)^B25-(1+B21)^B25)/(B22-B21)</f>
-        <v>447778.03896473994</v>
+        <v>779235.42589526367</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>8</v>
       </c>
-      <c r="B96" s="74"/>
+      <c r="B96" s="64"/>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>91</v>
-      </c>
-      <c r="B97" s="6">
+        <v>90</v>
+      </c>
+      <c r="B97" s="5">
         <f>B36*B35*(1+B22)^B25</f>
-        <v>3731.4833418175972</v>
+        <v>7978.4538410338864</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
         <v>36</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="5">
         <f>B35</f>
-        <v>3061.1160154725289</v>
+        <v>4055.8413624190966</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B99" s="48">
+        <v>91</v>
+      </c>
+      <c r="B99" s="42">
         <f>B95-B96+B97-B98</f>
-        <v>448448.406291085</v>
+        <v>783158.03837387846</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
         <v>81</v>
       </c>
-      <c r="B101" s="12"/>
+      <c r="B101" s="10"/>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>94</v>
-      </c>
-      <c r="B103" s="72">
+        <v>93</v>
+      </c>
+      <c r="B103" s="13">
         <f>B89+B93+B99+B101</f>
-        <v>568448.40629108506</v>
+        <v>903158.03837387846</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>97</v>
-      </c>
-      <c r="B105" s="72">
+        <v>96</v>
+      </c>
+      <c r="B105" s="13">
         <f>B37*B25+B69*((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)/(B22-B21)</f>
-        <v>568448.40629108495</v>
+        <v>903158.03837387834</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
         <v>62</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B106" s="5">
         <f>B37*B25</f>
         <v>120000</v>
       </c>
@@ -2684,56 +2676,56 @@
       <c r="A107" t="s">
         <v>8</v>
       </c>
-      <c r="B107" s="6">
+      <c r="B107" s="5">
         <f>B69</f>
-        <v>36733.392185670345</v>
+        <v>48670.096349029162</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>98</v>
-      </c>
-      <c r="B108" s="78">
+        <v>97</v>
+      </c>
+      <c r="B108" s="68">
         <f>((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)</f>
-        <v>-1.2208194761549431E-8</v>
+        <v>0.80455770735939747</v>
       </c>
     </row>
     <row r="109" spans="1:2">
-      <c r="B109" s="6">
+      <c r="B109" s="5">
         <f>B106+B107*B108</f>
-        <v>119999.99955155159</v>
+        <v>159157.90113553588</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>96</v>
-      </c>
-      <c r="B113" s="72">
+        <v>95</v>
+      </c>
+      <c r="B113" s="13">
         <f>(G37-B106)*(B22-B21)</f>
-        <v>-4.4844840605504148E-4</v>
+        <v>39157.901135535882</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>100</v>
-      </c>
-      <c r="B114" s="75">
+        <v>99</v>
+      </c>
+      <c r="B114" s="65">
         <f>((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)</f>
-        <v>-1.2208194761549431E-8</v>
+        <v>0.80455770735939747</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>99</v>
-      </c>
-      <c r="B116" s="6">
+        <v>98</v>
+      </c>
+      <c r="B116" s="5">
         <f>(G37-B106)*(B22-B21)/((1+B22)*((1+B22)^B25-(1+B21)^B25)+(B22-B21)*B36/12*(1+B22)^B25-(B22-B21)*B36/12)/12</f>
-        <v>3061.1160154725289</v>
+        <v>4055.8413624190966</v>
       </c>
     </row>
   </sheetData>
@@ -2752,46 +2744,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="39.375" customWidth="1"/>
-    <col min="2" max="2" width="17.625" customWidth="1"/>
+    <col min="1" max="1" width="39.3984375" customWidth="1"/>
+    <col min="2" max="2" width="17.59765625" customWidth="1"/>
     <col min="5" max="5" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="71"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="9" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="70"/>
-      <c r="B4" s="70"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2805,7 +2797,9 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="5">
+        <v>10000</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
@@ -2817,7 +2811,7 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <f>B6*B8</f>
         <v>150000</v>
       </c>
@@ -2843,34 +2837,34 @@
       <c r="E8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="49">
+      <c r="F8" s="43">
         <f>SUM(F5:F7)</f>
-        <v>150000</v>
+        <v>160000</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="80"/>
-      <c r="E10" s="18" t="s">
+      <c r="B10" s="71"/>
+      <c r="E10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="11" t="s">
+      <c r="B11" s="5">
+        <f>B6*(1-B8)</f>
+        <v>850000</v>
+      </c>
+      <c r="E11" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="4">
         <f>B16*(B11*B25-B11*(B17*(B25-1)*B25/2))</f>
-        <v>0</v>
+        <v>162434.99999999997</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2881,98 +2875,97 @@
         <f>1-B8</f>
         <v>0.85</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="72">
+      <c r="F12" s="13">
         <f>B6*B28*B25</f>
         <v>100000</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>0.03</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="72">
+      <c r="F13" s="13">
         <f>(B29)*B25</f>
         <v>240000</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="72">
+      <c r="F14" s="13">
         <f>B31*B25</f>
         <v>120000</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>0.3</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="72">
+      <c r="F15" s="13">
         <f>B30*B25</f>
         <v>120000</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="7">
-        <f>B13*0.7</f>
+      <c r="B16" s="6">
+        <f>B13*(1-B15)</f>
         <v>2.0999999999999998E-2</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="72">
+      <c r="F16" s="13">
         <f>SUM(F11:F15)</f>
-        <v>580000</v>
+        <v>742435</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <v>0.02</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="E18" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="80"/>
+      <c r="B19" s="71"/>
       <c r="E19" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <f>B8*B6*(1+B22)^B25-B6*B8</f>
-        <v>72036.642737751681</v>
+        <v>145072.70359343482</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2980,12 +2973,12 @@
         <v>5</v>
       </c>
       <c r="B20" s="2">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="E20" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <f>(B29+B31+B30+B28*B6)</f>
         <v>58000</v>
       </c>
@@ -2997,19 +2990,19 @@
       <c r="B21" s="2">
         <v>0.02</v>
       </c>
-      <c r="F21" s="12"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="1">
-        <v>0.04</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="48"/>
+      <c r="F22" s="42"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
@@ -3018,12 +3011,16 @@
       <c r="B23" s="1">
         <v>0.02</v>
       </c>
+      <c r="F23" s="77">
+        <f>F19+F20</f>
+        <v>203072.70359343482</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="15">
+      <c r="B24" s="12">
         <v>4.47E-3</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -3040,19 +3037,19 @@
       <c r="E25" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="80" t="s">
+      <c r="A26" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="80"/>
+      <c r="B26" s="71"/>
       <c r="E26" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <f>B6*(1+B20)^B25-B6</f>
-        <v>480244.28491834458</v>
+        <v>343916.37934412179</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3060,14 +3057,14 @@
         <v>9</v>
       </c>
       <c r="B27" s="1">
-        <v>0</v>
-      </c>
-      <c r="E27" s="5" t="s">
+        <v>0.01</v>
+      </c>
+      <c r="E27" t="s">
         <v>45</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <f>F26-F12</f>
-        <v>380244.28491834458</v>
+        <v>243916.37934412179</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3077,12 +3074,12 @@
       <c r="B28" s="1">
         <v>0.01</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="49">
+      <c r="F28" s="43">
         <f>F27*22/30*0.3</f>
-        <v>83653.742682035794</v>
+        <v>53661.603455706798</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3092,10 +3089,10 @@
       <c r="B29" s="4">
         <v>24000</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
@@ -3107,9 +3104,9 @@
       <c r="E30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="71">
+      <c r="F30" s="62">
         <f>F26-F28</f>
-        <v>396590.5422363088</v>
+        <v>290254.775888415</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3124,7 +3121,7 @@
       <c r="E32" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F32" s="49"/>
+      <c r="F32" s="43"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
@@ -3132,20 +3129,20 @@
       </c>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:6" ht="18">
+    <row r="34" spans="1:6" ht="17.399999999999999">
       <c r="A34" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="73">
+      <c r="B34" s="63">
         <f>F34/((1-(1+B21)^B25)/(1-(1+B21)))/12</f>
-        <v>3085.6653829440797</v>
+        <v>5763.1067169287517</v>
       </c>
       <c r="E34" t="s">
         <v>50</v>
       </c>
-      <c r="F34" s="72">
+      <c r="F34" s="13">
         <f>F8+F16+F19-F30</f>
-        <v>405446.10050144291</v>
+        <v>757252.92770501971</v>
       </c>
     </row>
     <row r="35" spans="1:6">

</xml_diff>